<commit_message>
more benchmarking, updated working hours
</commit_message>
<xml_diff>
--- a/Hours Stefan.xlsx
+++ b/Hours Stefan.xlsx
@@ -1216,7 +1216,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1225,7 +1228,7 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1234,13 +1237,10 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9663,385 +9663,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="58"/>
-      <c r="AE1" s="58"/>
-      <c r="AF1" s="58"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="58"/>
-      <c r="AI1" s="58"/>
-      <c r="AJ1" s="58"/>
-      <c r="AK1" s="58"/>
-      <c r="AL1" s="58"/>
-      <c r="AM1" s="58"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="58"/>
-      <c r="AQ1" s="58"/>
-      <c r="AR1" s="58"/>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="58"/>
-      <c r="AV1" s="58"/>
-      <c r="AW1" s="58"/>
-      <c r="AX1" s="58"/>
-      <c r="AY1" s="58"/>
-      <c r="AZ1" s="58"/>
-      <c r="BA1" s="58"/>
-      <c r="BB1" s="58"/>
-      <c r="BC1" s="58"/>
-      <c r="BD1" s="58"/>
-      <c r="BE1" s="58"/>
-      <c r="BF1" s="58"/>
-      <c r="BG1" s="58"/>
-      <c r="BH1" s="58"/>
-      <c r="BI1" s="58"/>
-      <c r="BJ1" s="58"/>
-      <c r="BK1" s="58"/>
-      <c r="BL1" s="58"/>
-      <c r="BM1" s="58"/>
-      <c r="BN1" s="58"/>
-      <c r="BO1" s="58"/>
-      <c r="BP1" s="58"/>
-      <c r="BQ1" s="58"/>
-      <c r="BR1" s="58"/>
-      <c r="BS1" s="58"/>
-      <c r="BT1" s="58"/>
-      <c r="BU1" s="58"/>
-      <c r="BV1" s="58"/>
-      <c r="BW1" s="58"/>
-      <c r="BX1" s="58"/>
-      <c r="BY1" s="58"/>
-      <c r="BZ1" s="58"/>
-      <c r="CA1" s="58"/>
-      <c r="CB1" s="58"/>
-      <c r="CC1" s="58"/>
-      <c r="CD1" s="58"/>
-      <c r="CE1" s="58"/>
-      <c r="CF1" s="58"/>
-      <c r="CG1" s="58"/>
-      <c r="CH1" s="58"/>
-      <c r="CI1" s="58"/>
-      <c r="CJ1" s="58"/>
-      <c r="CK1" s="58"/>
-      <c r="CL1" s="58"/>
-      <c r="CM1" s="58"/>
-      <c r="CN1" s="58"/>
-      <c r="CO1" s="58"/>
-      <c r="CP1" s="58"/>
-      <c r="CQ1" s="58"/>
-      <c r="CR1" s="58"/>
-      <c r="CS1" s="58"/>
-      <c r="CT1" s="58"/>
-      <c r="CU1" s="58"/>
-      <c r="CV1" s="58"/>
-      <c r="CW1" s="58"/>
-      <c r="CX1" s="58"/>
-      <c r="CY1" s="58"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="52"/>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
+      <c r="AK1" s="52"/>
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="52"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AQ1" s="52"/>
+      <c r="AR1" s="52"/>
+      <c r="AS1" s="52"/>
+      <c r="AT1" s="52"/>
+      <c r="AU1" s="52"/>
+      <c r="AV1" s="52"/>
+      <c r="AW1" s="52"/>
+      <c r="AX1" s="52"/>
+      <c r="AY1" s="52"/>
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="52"/>
+      <c r="BF1" s="52"/>
+      <c r="BG1" s="52"/>
+      <c r="BH1" s="52"/>
+      <c r="BI1" s="52"/>
+      <c r="BJ1" s="52"/>
+      <c r="BK1" s="52"/>
+      <c r="BL1" s="52"/>
+      <c r="BM1" s="52"/>
+      <c r="BN1" s="52"/>
+      <c r="BO1" s="52"/>
+      <c r="BP1" s="52"/>
+      <c r="BQ1" s="52"/>
+      <c r="BR1" s="52"/>
+      <c r="BS1" s="52"/>
+      <c r="BT1" s="52"/>
+      <c r="BU1" s="52"/>
+      <c r="BV1" s="52"/>
+      <c r="BW1" s="52"/>
+      <c r="BX1" s="52"/>
+      <c r="BY1" s="52"/>
+      <c r="BZ1" s="52"/>
+      <c r="CA1" s="52"/>
+      <c r="CB1" s="52"/>
+      <c r="CC1" s="52"/>
+      <c r="CD1" s="52"/>
+      <c r="CE1" s="52"/>
+      <c r="CF1" s="52"/>
+      <c r="CG1" s="52"/>
+      <c r="CH1" s="52"/>
+      <c r="CI1" s="52"/>
+      <c r="CJ1" s="52"/>
+      <c r="CK1" s="52"/>
+      <c r="CL1" s="52"/>
+      <c r="CM1" s="52"/>
+      <c r="CN1" s="52"/>
+      <c r="CO1" s="52"/>
+      <c r="CP1" s="52"/>
+      <c r="CQ1" s="52"/>
+      <c r="CR1" s="52"/>
+      <c r="CS1" s="52"/>
+      <c r="CT1" s="52"/>
+      <c r="CU1" s="52"/>
+      <c r="CV1" s="52"/>
+      <c r="CW1" s="52"/>
+      <c r="CX1" s="52"/>
+      <c r="CY1" s="52"/>
       <c r="CZ1" s="11"/>
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="52" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="52" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="52" t="s">
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="52" t="s">
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
+      <c r="AF2" s="54"/>
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="55"/>
+      <c r="AI2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="52" t="s">
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="55"/>
+      <c r="AP2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="54"/>
-      <c r="AW2" s="52" t="s">
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="55"/>
+      <c r="AW2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="AX2" s="53"/>
-      <c r="AY2" s="53"/>
-      <c r="AZ2" s="53"/>
-      <c r="BA2" s="53"/>
-      <c r="BB2" s="53"/>
-      <c r="BC2" s="54"/>
-      <c r="BD2" s="52" t="s">
+      <c r="AX2" s="54"/>
+      <c r="AY2" s="54"/>
+      <c r="AZ2" s="54"/>
+      <c r="BA2" s="54"/>
+      <c r="BB2" s="54"/>
+      <c r="BC2" s="55"/>
+      <c r="BD2" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="BE2" s="53"/>
-      <c r="BF2" s="53"/>
-      <c r="BG2" s="53"/>
-      <c r="BH2" s="53"/>
-      <c r="BI2" s="53"/>
-      <c r="BJ2" s="54"/>
-      <c r="BK2" s="52" t="s">
+      <c r="BE2" s="54"/>
+      <c r="BF2" s="54"/>
+      <c r="BG2" s="54"/>
+      <c r="BH2" s="54"/>
+      <c r="BI2" s="54"/>
+      <c r="BJ2" s="55"/>
+      <c r="BK2" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="54"/>
-      <c r="BR2" s="52" t="s">
+      <c r="BL2" s="54"/>
+      <c r="BM2" s="54"/>
+      <c r="BN2" s="54"/>
+      <c r="BO2" s="54"/>
+      <c r="BP2" s="54"/>
+      <c r="BQ2" s="55"/>
+      <c r="BR2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
-      <c r="BX2" s="54"/>
-      <c r="BY2" s="52" t="s">
+      <c r="BS2" s="54"/>
+      <c r="BT2" s="54"/>
+      <c r="BU2" s="54"/>
+      <c r="BV2" s="54"/>
+      <c r="BW2" s="54"/>
+      <c r="BX2" s="55"/>
+      <c r="BY2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="BZ2" s="53"/>
-      <c r="CA2" s="53"/>
-      <c r="CB2" s="53"/>
-      <c r="CC2" s="53"/>
-      <c r="CD2" s="53"/>
-      <c r="CE2" s="54"/>
-      <c r="CF2" s="52" t="s">
+      <c r="BZ2" s="54"/>
+      <c r="CA2" s="54"/>
+      <c r="CB2" s="54"/>
+      <c r="CC2" s="54"/>
+      <c r="CD2" s="54"/>
+      <c r="CE2" s="55"/>
+      <c r="CF2" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="CG2" s="53"/>
-      <c r="CH2" s="53"/>
-      <c r="CI2" s="53"/>
-      <c r="CJ2" s="53"/>
-      <c r="CK2" s="53"/>
-      <c r="CL2" s="54"/>
-      <c r="CM2" s="52" t="s">
+      <c r="CG2" s="54"/>
+      <c r="CH2" s="54"/>
+      <c r="CI2" s="54"/>
+      <c r="CJ2" s="54"/>
+      <c r="CK2" s="54"/>
+      <c r="CL2" s="55"/>
+      <c r="CM2" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="CN2" s="53"/>
-      <c r="CO2" s="53"/>
-      <c r="CP2" s="53"/>
-      <c r="CQ2" s="53"/>
-      <c r="CR2" s="53"/>
-      <c r="CS2" s="54"/>
-      <c r="CT2" s="52" t="s">
+      <c r="CN2" s="54"/>
+      <c r="CO2" s="54"/>
+      <c r="CP2" s="54"/>
+      <c r="CQ2" s="54"/>
+      <c r="CR2" s="54"/>
+      <c r="CS2" s="55"/>
+      <c r="CT2" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="CU2" s="53"/>
-      <c r="CV2" s="53"/>
-      <c r="CW2" s="53"/>
-      <c r="CX2" s="53"/>
-      <c r="CY2" s="53"/>
-      <c r="CZ2" s="54"/>
+      <c r="CU2" s="54"/>
+      <c r="CV2" s="54"/>
+      <c r="CW2" s="54"/>
+      <c r="CX2" s="54"/>
+      <c r="CY2" s="54"/>
+      <c r="CZ2" s="55"/>
     </row>
     <row r="3" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="G3" s="60">
+      <c r="G3" s="56">
         <f>G5</f>
         <v>42107</v>
       </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="55">
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="60">
         <f>N5</f>
         <v>42114</v>
       </c>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="55">
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="60">
         <f>U5</f>
         <v>42121</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="57"/>
-      <c r="AB3" s="55">
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="60">
         <f>AB5</f>
         <v>42128</v>
       </c>
-      <c r="AC3" s="56"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="56"/>
-      <c r="AF3" s="56"/>
-      <c r="AG3" s="56"/>
-      <c r="AH3" s="57"/>
-      <c r="AI3" s="55">
+      <c r="AC3" s="57"/>
+      <c r="AD3" s="57"/>
+      <c r="AE3" s="57"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="60">
         <f>AI5</f>
         <v>42135</v>
       </c>
-      <c r="AJ3" s="56"/>
-      <c r="AK3" s="56"/>
-      <c r="AL3" s="56"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="57"/>
-      <c r="AP3" s="55">
+      <c r="AJ3" s="57"/>
+      <c r="AK3" s="57"/>
+      <c r="AL3" s="57"/>
+      <c r="AM3" s="57"/>
+      <c r="AN3" s="57"/>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="60">
         <f>AP5</f>
         <v>42142</v>
       </c>
-      <c r="AQ3" s="56"/>
-      <c r="AR3" s="56"/>
-      <c r="AS3" s="56"/>
-      <c r="AT3" s="56"/>
-      <c r="AU3" s="56"/>
-      <c r="AV3" s="57"/>
-      <c r="AW3" s="55">
+      <c r="AQ3" s="57"/>
+      <c r="AR3" s="57"/>
+      <c r="AS3" s="57"/>
+      <c r="AT3" s="57"/>
+      <c r="AU3" s="57"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="60">
         <f t="shared" ref="AW3" si="0">AW5</f>
         <v>42149</v>
       </c>
-      <c r="AX3" s="56"/>
-      <c r="AY3" s="56"/>
-      <c r="AZ3" s="56"/>
-      <c r="BA3" s="56"/>
-      <c r="BB3" s="56"/>
-      <c r="BC3" s="57"/>
-      <c r="BD3" s="55">
+      <c r="AX3" s="57"/>
+      <c r="AY3" s="57"/>
+      <c r="AZ3" s="57"/>
+      <c r="BA3" s="57"/>
+      <c r="BB3" s="57"/>
+      <c r="BC3" s="58"/>
+      <c r="BD3" s="60">
         <f t="shared" ref="BD3" si="1">BD5</f>
         <v>42156</v>
       </c>
-      <c r="BE3" s="56"/>
-      <c r="BF3" s="56"/>
-      <c r="BG3" s="56"/>
-      <c r="BH3" s="56"/>
-      <c r="BI3" s="56"/>
-      <c r="BJ3" s="57"/>
-      <c r="BK3" s="55">
+      <c r="BE3" s="57"/>
+      <c r="BF3" s="57"/>
+      <c r="BG3" s="57"/>
+      <c r="BH3" s="57"/>
+      <c r="BI3" s="57"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="60">
         <f t="shared" ref="BK3" si="2">BK5</f>
         <v>42163</v>
       </c>
-      <c r="BL3" s="56"/>
-      <c r="BM3" s="56"/>
-      <c r="BN3" s="56"/>
-      <c r="BO3" s="56"/>
-      <c r="BP3" s="56"/>
-      <c r="BQ3" s="57"/>
-      <c r="BR3" s="55">
+      <c r="BL3" s="57"/>
+      <c r="BM3" s="57"/>
+      <c r="BN3" s="57"/>
+      <c r="BO3" s="57"/>
+      <c r="BP3" s="57"/>
+      <c r="BQ3" s="58"/>
+      <c r="BR3" s="60">
         <f t="shared" ref="BR3" si="3">BR5</f>
         <v>42170</v>
       </c>
-      <c r="BS3" s="56"/>
-      <c r="BT3" s="56"/>
-      <c r="BU3" s="56"/>
-      <c r="BV3" s="56"/>
-      <c r="BW3" s="56"/>
-      <c r="BX3" s="57"/>
-      <c r="BY3" s="55">
+      <c r="BS3" s="57"/>
+      <c r="BT3" s="57"/>
+      <c r="BU3" s="57"/>
+      <c r="BV3" s="57"/>
+      <c r="BW3" s="57"/>
+      <c r="BX3" s="58"/>
+      <c r="BY3" s="60">
         <f t="shared" ref="BY3" si="4">BY5</f>
         <v>42177</v>
       </c>
-      <c r="BZ3" s="56"/>
-      <c r="CA3" s="56"/>
-      <c r="CB3" s="56"/>
-      <c r="CC3" s="56"/>
-      <c r="CD3" s="56"/>
-      <c r="CE3" s="57"/>
-      <c r="CF3" s="55">
+      <c r="BZ3" s="57"/>
+      <c r="CA3" s="57"/>
+      <c r="CB3" s="57"/>
+      <c r="CC3" s="57"/>
+      <c r="CD3" s="57"/>
+      <c r="CE3" s="58"/>
+      <c r="CF3" s="60">
         <f t="shared" ref="CF3" si="5">CF5</f>
         <v>42184</v>
       </c>
-      <c r="CG3" s="56"/>
-      <c r="CH3" s="56"/>
-      <c r="CI3" s="56"/>
-      <c r="CJ3" s="56"/>
-      <c r="CK3" s="56"/>
-      <c r="CL3" s="57"/>
-      <c r="CM3" s="55">
+      <c r="CG3" s="57"/>
+      <c r="CH3" s="57"/>
+      <c r="CI3" s="57"/>
+      <c r="CJ3" s="57"/>
+      <c r="CK3" s="57"/>
+      <c r="CL3" s="58"/>
+      <c r="CM3" s="60">
         <f t="shared" ref="CM3" si="6">CM5</f>
         <v>42191</v>
       </c>
-      <c r="CN3" s="56"/>
-      <c r="CO3" s="56"/>
-      <c r="CP3" s="56"/>
-      <c r="CQ3" s="56"/>
-      <c r="CR3" s="56"/>
-      <c r="CS3" s="57"/>
-      <c r="CT3" s="55">
+      <c r="CN3" s="57"/>
+      <c r="CO3" s="57"/>
+      <c r="CP3" s="57"/>
+      <c r="CQ3" s="57"/>
+      <c r="CR3" s="57"/>
+      <c r="CS3" s="58"/>
+      <c r="CT3" s="60">
         <f t="shared" ref="CT3" si="7">CT5</f>
         <v>42198</v>
       </c>
-      <c r="CU3" s="56"/>
-      <c r="CV3" s="56"/>
-      <c r="CW3" s="56"/>
-      <c r="CX3" s="56"/>
-      <c r="CY3" s="56"/>
-      <c r="CZ3" s="57"/>
+      <c r="CU3" s="57"/>
+      <c r="CV3" s="57"/>
+      <c r="CW3" s="57"/>
+      <c r="CX3" s="57"/>
+      <c r="CY3" s="57"/>
+      <c r="CZ3" s="58"/>
     </row>
     <row r="4" spans="1:104" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -22562,6 +22562,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="CM3:CS3"/>
+    <mergeCell ref="CT3:CZ3"/>
+    <mergeCell ref="BY2:CE2"/>
+    <mergeCell ref="CF2:CL2"/>
+    <mergeCell ref="BY3:CE3"/>
+    <mergeCell ref="CF3:CL3"/>
+    <mergeCell ref="CM2:CS2"/>
+    <mergeCell ref="BD3:BJ3"/>
+    <mergeCell ref="BK2:BQ2"/>
+    <mergeCell ref="BR2:BX2"/>
+    <mergeCell ref="BK3:BQ3"/>
+    <mergeCell ref="BR3:BX3"/>
     <mergeCell ref="A1:CY1"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="G3:M3"/>
@@ -22578,19 +22591,6 @@
     <mergeCell ref="AI3:AO3"/>
     <mergeCell ref="AP3:AV3"/>
     <mergeCell ref="AW3:BC3"/>
-    <mergeCell ref="BD3:BJ3"/>
-    <mergeCell ref="BK2:BQ2"/>
-    <mergeCell ref="BR2:BX2"/>
-    <mergeCell ref="BK3:BQ3"/>
-    <mergeCell ref="BR3:BX3"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="CM3:CS3"/>
-    <mergeCell ref="CT3:CZ3"/>
-    <mergeCell ref="BY2:CE2"/>
-    <mergeCell ref="CF2:CL2"/>
-    <mergeCell ref="BY3:CE3"/>
-    <mergeCell ref="CF3:CL3"/>
-    <mergeCell ref="CM2:CS2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:CW300">
     <cfRule type="expression" dxfId="14" priority="77">
@@ -45955,7 +45955,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45995,7 +45995,7 @@
       </c>
       <c r="H3">
         <f>SUM(Table1345[Time Spent (hours)])</f>
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -46355,7 +46355,7 @@
         <v>250</v>
       </c>
       <c r="B36">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
         <v>249</v>

</xml_diff>